<commit_message>
Updated code, steps + uploaded video for smart irrigation(moisture)
</commit_message>
<xml_diff>
--- a/Water/Moisture based smart irrigation/moisture_based_smart_irrigation_master.xlsx
+++ b/Water/Moisture based smart irrigation/moisture_based_smart_irrigation_master.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t>Objective</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Updated</t>
   </si>
   <si>
-    <t>Pending</t>
-  </si>
-  <si>
     <t>Images</t>
   </si>
   <si>
@@ -132,16 +129,22 @@
     <t>Connect relay to pump</t>
   </si>
   <si>
-    <t>4//6</t>
-  </si>
-  <si>
-    <t>4//5</t>
-  </si>
-  <si>
     <t>Working video</t>
   </si>
   <si>
     <t>Code modified to include connections and parameters</t>
+  </si>
+  <si>
+    <t>5//5</t>
+  </si>
+  <si>
+    <t>6//6</t>
+  </si>
+  <si>
+    <t>Upload code</t>
+  </si>
+  <si>
+    <t>Not sure how to frame steps?</t>
   </si>
 </sst>
 </file>
@@ -165,7 +168,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,6 +187,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -197,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -208,6 +217,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,15 +556,15 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
         <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>39</v>
@@ -562,18 +572,18 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>38</v>
+        <v>14</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -587,7 +597,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,7 +623,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -624,7 +634,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -632,10 +642,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
         <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -650,7 +660,7 @@
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -672,7 +682,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,13 +695,13 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D1" s="4"/>
     </row>
@@ -700,10 +710,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -711,25 +721,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
         <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="6"/>
     </row>
@@ -738,25 +748,25 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -764,44 +774,47 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>5</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>5</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>37</v>
+      <c r="C15" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="2">
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UPdated moisture based smart irrigation
</commit_message>
<xml_diff>
--- a/Water/Moisture based smart irrigation/moisture_based_smart_irrigation_master.xlsx
+++ b/Water/Moisture based smart irrigation/moisture_based_smart_irrigation_master.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="Components" sheetId="2" r:id="rId2"/>
     <sheet name="Steps" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="72">
   <si>
     <t>Objective</t>
   </si>
@@ -88,9 +87,6 @@
     <t>Sl no.</t>
   </si>
   <si>
-    <t>5V and GND Connections</t>
-  </si>
-  <si>
     <t>Connect soil moisture sensor to Arduino UNO</t>
   </si>
   <si>
@@ -160,12 +156,6 @@
     <t>Relay contacts(3)-Normally open(NO),Normally closed(NC),Common(COM)</t>
   </si>
   <si>
-    <t>COM to pump</t>
-  </si>
-  <si>
-    <t>NC to power supply</t>
-  </si>
-  <si>
     <t>Final code</t>
   </si>
   <si>
@@ -175,12 +165,6 @@
     <t>Breadboard connections</t>
   </si>
   <si>
-    <t>Soil moisture sensor uses the property of resistance to measure moisture content of the soil. More the water content, more the conductivity between the probes and so lower the resistance offered. So a low signal is transmitted. Similarly, lesser the water content, high signal is transmitted.</t>
-  </si>
-  <si>
-    <t>Soil moisture sensor pins(4)-Vcc,GND,analog pin A0, digital pin D0</t>
-  </si>
-  <si>
     <t>Flow meter pins(3)- Vcc, GND, data pin</t>
   </si>
   <si>
@@ -190,9 +174,6 @@
     <t>Attach flow sensor to tap</t>
   </si>
   <si>
-    <t>The flow sensor contains an integrated magnetic hall effect sensor that outputs an electrical pulse with every revolution.</t>
-  </si>
-  <si>
     <t>The flow sensor sits in line with the water flow such that the arrow on it indicates the direction of flow.</t>
   </si>
   <si>
@@ -212,6 +193,45 @@
   </si>
   <si>
     <t>2 sub codes</t>
+  </si>
+  <si>
+    <t>How The Sensor Works: Soil moisture sensor uses the property of resistance to measure moisture content of the soil. More the water content, more the conductivity between the probes and so lower the resistance offered. So a low signal is transmitted. Similarly, lesser the water content, high signal is transmitted.</t>
+  </si>
+  <si>
+    <t>Setup Breadboard: 5V and GND Connections</t>
+  </si>
+  <si>
+    <t>Soil moisture sensor pins(4)-Vcc,GND,analog pin A0, digital pin D0 (WE will NOT use D0)</t>
+  </si>
+  <si>
+    <t>How The Sensor Works: The flow sensor contains an integrated magnetic hall effect sensor that outputs an electrical pulse with every revolution.</t>
+  </si>
+  <si>
+    <t>COM to power Supply</t>
+  </si>
+  <si>
+    <t>NC to pump</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Vendor Link</t>
+  </si>
+  <si>
+    <t>Here</t>
+  </si>
+  <si>
+    <t>Box</t>
+  </si>
+  <si>
+    <t>Casing</t>
+  </si>
+  <si>
+    <t>Power Adaptor</t>
+  </si>
+  <si>
+    <t>Power</t>
   </si>
 </sst>
 </file>
@@ -303,7 +323,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -341,6 +361,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -402,7 +423,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -437,7 +458,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -648,14 +669,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -679,7 +700,7 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -695,7 +716,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -703,12 +724,12 @@
         <v>14</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
@@ -722,28 +743,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -753,8 +780,14 @@
       <c r="C2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>150</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -764,8 +797,14 @@
       <c r="C3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>357</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -775,32 +814,97 @@
       <c r="C4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <f>124+75</f>
+        <v>199</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>470</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>150</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
+      <c r="D7">
+        <v>480</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8">
+        <f>490+60</f>
+        <v>550</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9">
+        <f>140+76</f>
+        <v>216</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E5" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="E4" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E7" r:id="rId6"/>
+    <hyperlink ref="E8" r:id="rId7"/>
+    <hyperlink ref="E9" r:id="rId8"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -809,20 +913,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.33203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
@@ -833,124 +937,124 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="C3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="C4" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C4" s="12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C6" s="12" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="C7" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C8" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C9" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="C10" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="C12" s="12" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="C13" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="C14" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C15" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="C16" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -958,60 +1062,60 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="C18" s="18" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="C19" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C20" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E20" s="10"/>
     </row>
     <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C21" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="C22" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>5</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="19" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="11"/>
@@ -1021,20 +1125,20 @@
         <v>6</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="19" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="11"/>
@@ -1044,65 +1148,68 @@
         <v>7</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E27" s="20"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
       <c r="C28" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="11"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B29" s="5"/>
       <c r="C29" s="19" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="11"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B30" s="5"/>
       <c r="C30" s="19" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="11"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>8</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" s="16"/>
       <c r="D31" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>9</v>
       </c>
       <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="13" t="s">
-        <v>36</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created folder and excel for each sol
</commit_message>
<xml_diff>
--- a/Water/Moisture based smart irrigation/moisture_based_smart_irrigation_master.xlsx
+++ b/Water/Moisture based smart irrigation/moisture_based_smart_irrigation_master.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="70">
   <si>
     <t>Objective</t>
   </si>
@@ -69,12 +69,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>flow based</t>
-  </si>
-  <si>
-    <t>moisture based</t>
-  </si>
-  <si>
     <t>Sl no.</t>
   </si>
   <si>
@@ -229,6 +223,9 @@
   </si>
   <si>
     <t>Based on moisture content of the soil and required moisture for plant, water is supplied as and when needed.</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -281,7 +278,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -300,12 +297,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -320,7 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -329,7 +320,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -667,7 +657,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,8 +676,8 @@
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>70</v>
+      <c r="B2" s="11" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
@@ -706,7 +696,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
@@ -721,21 +711,21 @@
       <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>54</v>
+      <c r="B6" s="8" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>53</v>
+      <c r="B7" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -749,135 +739,138 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2">
+      <c r="C2">
         <v>150</v>
       </c>
-      <c r="E2" s="21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2" s="20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3">
+      <c r="C3">
         <v>357</v>
       </c>
-      <c r="E3" s="21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3" s="20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="D4">
+      <c r="C4">
         <v>470</v>
       </c>
-      <c r="E4" s="21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4" s="20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D5">
+      <c r="C5">
         <v>150</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="D5" s="20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>66</v>
-      </c>
       <c r="B6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6">
+        <v>63</v>
+      </c>
+      <c r="C6">
         <f>490+60</f>
         <v>550</v>
       </c>
-      <c r="E6" s="21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6" s="20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7">
+        <v>65</v>
+      </c>
+      <c r="C7">
         <f>140+76</f>
         <v>216</v>
       </c>
-      <c r="E7" s="21" t="s">
-        <v>64</v>
+      <c r="D7" s="20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="1">
+        <f>SUM(C2:C8)</f>
+        <v>1893</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="E6" r:id="rId5"/>
-    <hyperlink ref="E7" r:id="rId6"/>
+    <hyperlink ref="D4" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -885,34 +878,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.28515625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -920,26 +913,26 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>45</v>
+        <v>55</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C3" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>44</v>
+      <c r="C3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C4" s="12" t="s">
-        <v>34</v>
+      <c r="C4" s="11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="105" x14ac:dyDescent="0.25">
@@ -947,42 +940,42 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C6" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="C6" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="12" t="s">
-        <v>21</v>
+      <c r="C7" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="C9" s="11" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="C9" s="12" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
-      <c r="C10" s="15" t="s">
-        <v>22</v>
+      <c r="C10" s="14" t="s">
+        <v>20</v>
       </c>
       <c r="E10" s="6"/>
     </row>
@@ -991,42 +984,42 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C12" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="21" t="s">
+      <c r="C12" s="11" t="s">
         <v>44</v>
       </c>
+      <c r="D12" s="20" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="12" t="s">
-        <v>21</v>
+      <c r="C13" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="C14" s="12" t="s">
+      <c r="A14" s="16"/>
+      <c r="C14" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="C15" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="C15" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="12" t="s">
-        <v>24</v>
+      <c r="C16" s="11" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1034,39 +1027,39 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>44</v>
+        <v>23</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="18" t="s">
-        <v>47</v>
+      <c r="C18" s="17" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="12" t="s">
-        <v>21</v>
+      <c r="C19" s="11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="C21" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="10"/>
-    </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="C21" s="12" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="12" t="s">
-        <v>26</v>
+      <c r="C22" s="11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1074,103 +1067,103 @@
         <v>5</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" s="11"/>
+        <v>48</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="10"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
-      <c r="C24" s="19" t="s">
-        <v>52</v>
+      <c r="C24" s="18" t="s">
+        <v>50</v>
       </c>
       <c r="D24" s="6"/>
-      <c r="E24" s="11"/>
+      <c r="E24" s="10"/>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>6</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E25" s="11"/>
+        <v>46</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="10"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
-      <c r="C26" s="19" t="s">
-        <v>52</v>
+      <c r="C26" s="18" t="s">
+        <v>50</v>
       </c>
       <c r="D26" s="6"/>
-      <c r="E26" s="11"/>
+      <c r="E26" s="10"/>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>7</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="20"/>
+      <c r="E27" s="19"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
-      <c r="C28" s="19" t="s">
-        <v>21</v>
+      <c r="C28" s="18" t="s">
+        <v>19</v>
       </c>
       <c r="D28" s="4"/>
-      <c r="E28" s="11"/>
+      <c r="E28" s="10"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
-      <c r="C29" s="19" t="s">
-        <v>60</v>
+      <c r="C29" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="D29" s="4"/>
-      <c r="E29" s="11"/>
+      <c r="E29" s="10"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
-      <c r="C30" s="19" t="s">
-        <v>61</v>
+      <c r="C30" s="18" t="s">
+        <v>59</v>
       </c>
       <c r="D30" s="4"/>
-      <c r="E30" s="11"/>
+      <c r="E30" s="10"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>8</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="11" t="s">
-        <v>43</v>
+        <v>27</v>
+      </c>
+      <c r="C31" s="15"/>
+      <c r="D31" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="11" t="s">
-        <v>69</v>
+      <c r="C32" s="15"/>
+      <c r="D32" s="10" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1178,10 +1171,10 @@
         <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>32</v>
+        <v>29</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated water meter diy2
</commit_message>
<xml_diff>
--- a/Water/Moisture based smart irrigation/moisture_based_smart_irrigation_master.xlsx
+++ b/Water/Moisture based smart irrigation/moisture_based_smart_irrigation_master.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="78">
   <si>
     <t>Objective</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Connect GND from Arduino UNO to breadboard</t>
   </si>
   <si>
-    <t>Each hole in the breadboard is connected to metal strips underneath. These metal strips are shown in the image. For series connection, connect holes in the same metal strip.</t>
-  </si>
-  <si>
     <t>Attachments</t>
   </si>
   <si>
@@ -177,9 +174,6 @@
     <t>7/8</t>
   </si>
   <si>
-    <t>2 sub codes</t>
-  </si>
-  <si>
     <t>How The Sensor Works: Soil moisture sensor uses the property of resistance to measure moisture content of the soil. More the water content, more the conductivity between the probes and so lower the resistance offered. So a low signal is transmitted. Similarly, lesser the water content, high signal is transmitted.</t>
   </si>
   <si>
@@ -226,6 +220,36 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Each hole in the breadboard is connected by metal strips underneath the plastic. These connections are shown in the image. For series connection(same signal given to multiple pins at once), place jumper cables into holes in the same line.</t>
+  </si>
+  <si>
+    <t>Small or large breadboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Breadboard is divided into two halves by a ridge to ensure no cross-connection between the halves. If you are a beginner and just want to get the output, connect 5V to A1 on line 1 and connect GND to A5 on line 5. Place any 5V or Vcc connections in line 1,and any GND connections in line 5. </t>
+  </si>
+  <si>
+    <t>code atached</t>
+  </si>
+  <si>
+    <t>we want pump off and only when triggered on</t>
+  </si>
+  <si>
+    <t>ip56 enclosure</t>
+  </si>
+  <si>
+    <t>Upload</t>
+  </si>
+  <si>
+    <t>Git</t>
+  </si>
+  <si>
+    <t>Instructable</t>
+  </si>
+  <si>
+    <t>2 codes+final</t>
   </si>
 </sst>
 </file>
@@ -654,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,7 +701,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
@@ -696,7 +720,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
@@ -712,7 +736,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
@@ -720,7 +744,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.25">
@@ -729,6 +753,19 @@
       </c>
       <c r="B8" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -741,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,10 +796,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -776,7 +813,7 @@
         <v>150</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -790,7 +827,7 @@
         <v>357</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -804,7 +841,7 @@
         <v>470</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -818,42 +855,42 @@
         <v>150</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C6">
         <f>490+60</f>
         <v>550</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C7">
         <f>140+76</f>
         <v>216</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C9" s="1">
         <f>SUM(C2:C8)</f>
@@ -876,10 +913,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,24 +939,27 @@
         <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -927,7 +967,7 @@
         <v>31</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -943,15 +983,15 @@
         <v>18</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C6" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D6" s="20" t="s">
         <v>10</v>
@@ -964,12 +1004,12 @@
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C8" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C9" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -987,7 +1027,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>10</v>
@@ -995,10 +1035,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C12" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1009,12 +1049,12 @@
     <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
       <c r="C14" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C15" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1030,15 +1070,15 @@
         <v>23</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C18" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1048,13 +1088,13 @@
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C20" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C21" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1067,20 +1107,20 @@
         <v>5</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="18" t="s">
-        <v>49</v>
-      </c>
       <c r="D23" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E23" s="10"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="10"/>
@@ -1090,20 +1130,20 @@
         <v>6</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="18" t="s">
-        <v>47</v>
-      </c>
       <c r="D25" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E25" s="10"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="10"/>
@@ -1116,10 +1156,10 @@
         <v>25</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E27" s="19"/>
     </row>
@@ -1134,7 +1174,7 @@
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="10"/>
@@ -1142,7 +1182,7 @@
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
       <c r="C30" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="10"/>
@@ -1156,17 +1196,17 @@
       </c>
       <c r="C31" s="15"/>
       <c r="D31" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="15"/>
       <c r="D32" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>9</v>
       </c>
@@ -1175,6 +1215,29 @@
       </c>
       <c r="C33" s="12" t="s">
         <v>30</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="C35" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C37" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="11" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1191,8 +1254,9 @@
     <hyperlink ref="D27" r:id="rId10"/>
     <hyperlink ref="D31" r:id="rId11"/>
     <hyperlink ref="D32" r:id="rId12"/>
+    <hyperlink ref="D33" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>